<commit_message>
there will be blood
</commit_message>
<xml_diff>
--- a/movie_list.xlsx
+++ b/movie_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6084" uniqueCount="3573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6106" uniqueCount="3587">
   <si>
     <t xml:space="preserve">Tag</t>
   </si>
@@ -9868,6 +9868,48 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.themoviedb.org/t/p/w600_and_h900_bestv2/5M0j0B18abtBI5gi2RhfjjurTqb.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there_will_be_blood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There Will Be Blood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2h 38m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul Thomas Anderson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel Day-Lewis, Paul Dano, Ciarán Hinds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A story of family, religion, hatred, oil and madness, focusing on a turn-of-the-century prospector in the early days of the business.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/FeSLPELpMeM?si=HBmM3L7nAy4c-0nX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;iframe width="100%" height="250" src="https://www.youtube.com/embed/FeSLPELpMeM?si=HBmM3L7nAy4c-0nX" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.imdb.com/title/tt0469494/?ref_=nv_sr_srsg_0_tt_8_nm_0_in_0_q_there%2520will%2520b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Critics 91% / Audience 86%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.rottentomatoes.com/m/there_will_be_blood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.rogerebert.com/reviews/there-will-be-blood-2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.5/4 - Watching the movie is like viewing a natural disaster that you cannot turn away from. By that I do not mean that the movie is bad, any more than it is good. It is a force beyond categories. It has scenes of terror and poignancy, scenes of ruthless chicanery, scenes awesome for their scope, moments echoing with whispers and an ending that in some peculiar way this material demands, because it could not conclude on an appropriate note — there has been nothing appropriate about it. Those who hate the ending, and there may be many, might be asked to dictate a different one. Something bittersweet, perhaps? Grandly tragic? Only madness can supply a termination for this story.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://image.tmdb.org/t/p/w600_and_h900_bestv2/4ayObDELZfIXxVviT4GKTNc81wl.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">the_thing_from_another_world</t>
@@ -11066,10 +11108,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BO286"/>
+  <dimension ref="A1:BO287"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A226" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O237" activeCellId="0" sqref="O237"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A251" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D258" activeCellId="0" sqref="D258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.90234375" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16012,7 +16054,7 @@
         <v>998</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>29</v>
+        <v>684</v>
       </c>
       <c r="J68" s="5" t="s">
         <v>999</v>
@@ -25562,7 +25604,7 @@
       </c>
       <c r="X200" s="5"/>
     </row>
-    <row r="201" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="311.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
         <v>2618</v>
       </c>
@@ -29677,97 +29719,97 @@
         <v>25</v>
       </c>
       <c r="D258" s="5" t="s">
-        <v>3282</v>
+        <v>26</v>
       </c>
       <c r="E258" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F258" s="5" t="n">
-        <v>1951</v>
+        <v>2007</v>
       </c>
       <c r="G258" s="5" t="s">
-        <v>134</v>
+        <v>27</v>
       </c>
       <c r="H258" s="5" t="s">
-        <v>3283</v>
+        <v>3282</v>
       </c>
       <c r="I258" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J258" s="5" t="s">
-        <v>200</v>
+        <v>2496</v>
       </c>
       <c r="K258" s="5" t="s">
+        <v>3283</v>
+      </c>
+      <c r="L258" s="5" t="s">
         <v>3284</v>
       </c>
-      <c r="L258" s="5" t="s">
+      <c r="M258" s="5" t="s">
         <v>3285</v>
       </c>
-      <c r="M258" s="5" t="s">
+      <c r="N258" s="5" t="s">
         <v>3286</v>
       </c>
-      <c r="N258" s="5" t="s">
+      <c r="O258" s="5" t="s">
         <v>3287</v>
       </c>
-      <c r="O258" s="5" t="s">
+      <c r="P258" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="Q258" s="5" t="s">
         <v>3288</v>
       </c>
-      <c r="P258" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q258" s="5" t="s">
+      <c r="R258" s="5" t="s">
         <v>3289</v>
       </c>
-      <c r="R258" s="5" t="s">
+      <c r="S258" s="5" t="s">
         <v>3290</v>
       </c>
-      <c r="S258" s="5" t="s">
+      <c r="T258" s="5" t="s">
         <v>3291</v>
       </c>
-      <c r="T258" s="5" t="s">
+      <c r="U258" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="V258" s="5" t="s">
         <v>3292</v>
       </c>
-      <c r="U258" s="5" t="s">
+      <c r="W258" s="5" t="s">
         <v>3293</v>
-      </c>
-      <c r="V258" s="5" t="s">
-        <v>3294</v>
-      </c>
-      <c r="W258" s="5" t="s">
-        <v>3295</v>
       </c>
       <c r="X258" s="5"/>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="s">
-        <v>3296</v>
+        <v>3294</v>
       </c>
       <c r="B259" s="5" t="s">
-        <v>3282</v>
+        <v>3295</v>
       </c>
       <c r="C259" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D259" s="5" t="s">
-        <v>3282</v>
-      </c>
-      <c r="E259" s="10" t="s">
+        <v>3296</v>
+      </c>
+      <c r="E259" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F259" s="5" t="n">
-        <v>1982</v>
+        <v>1951</v>
       </c>
       <c r="G259" s="5" t="s">
-        <v>27</v>
+        <v>134</v>
       </c>
       <c r="H259" s="5" t="s">
-        <v>245</v>
+        <v>3297</v>
       </c>
       <c r="I259" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J259" s="5" t="s">
-        <v>3297</v>
+        <v>200</v>
       </c>
       <c r="K259" s="5" t="s">
         <v>3298</v>
@@ -29785,7 +29827,7 @@
         <v>3302</v>
       </c>
       <c r="P259" s="5" t="s">
-        <v>449</v>
+        <v>157</v>
       </c>
       <c r="Q259" s="5" t="s">
         <v>3303</v>
@@ -29800,154 +29842,154 @@
         <v>3306</v>
       </c>
       <c r="U259" s="5" t="s">
-        <v>41</v>
+        <v>3307</v>
       </c>
       <c r="V259" s="5" t="s">
-        <v>3307</v>
+        <v>3308</v>
       </c>
       <c r="W259" s="5" t="s">
-        <v>3308</v>
+        <v>3309</v>
       </c>
       <c r="X259" s="5"/>
     </row>
-    <row r="260" customFormat="false" ht="729.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="s">
-        <v>3309</v>
+        <v>3310</v>
       </c>
       <c r="B260" s="5" t="s">
-        <v>3282</v>
+        <v>3296</v>
       </c>
       <c r="C260" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D260" s="5" t="s">
-        <v>3282</v>
-      </c>
-      <c r="E260" s="6" t="s">
+        <v>3296</v>
+      </c>
+      <c r="E260" s="10" t="s">
         <v>26</v>
       </c>
       <c r="F260" s="5" t="n">
-        <v>2011</v>
+        <v>1982</v>
       </c>
       <c r="G260" s="5" t="s">
         <v>27</v>
       </c>
       <c r="H260" s="5" t="s">
-        <v>815</v>
+        <v>245</v>
       </c>
       <c r="I260" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J260" s="5" t="s">
-        <v>3297</v>
+        <v>3311</v>
       </c>
       <c r="K260" s="5" t="s">
-        <v>3310</v>
+        <v>3312</v>
       </c>
       <c r="L260" s="5" t="s">
-        <v>3311</v>
+        <v>3313</v>
       </c>
       <c r="M260" s="5" t="s">
-        <v>3312</v>
+        <v>3314</v>
       </c>
       <c r="N260" s="5" t="s">
-        <v>3313</v>
+        <v>3315</v>
       </c>
       <c r="O260" s="5" t="s">
-        <v>3314</v>
+        <v>3316</v>
       </c>
       <c r="P260" s="5" t="s">
-        <v>250</v>
+        <v>449</v>
       </c>
       <c r="Q260" s="5" t="s">
-        <v>3315</v>
+        <v>3317</v>
       </c>
       <c r="R260" s="5" t="s">
-        <v>3316</v>
+        <v>3318</v>
       </c>
       <c r="S260" s="5" t="s">
-        <v>3317</v>
+        <v>3319</v>
       </c>
       <c r="T260" s="5" t="s">
-        <v>3318</v>
+        <v>3320</v>
       </c>
       <c r="U260" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="V260" s="8" t="s">
-        <v>3319</v>
+      <c r="V260" s="5" t="s">
+        <v>3321</v>
       </c>
       <c r="W260" s="5" t="s">
-        <v>3320</v>
+        <v>3322</v>
       </c>
       <c r="X260" s="5"/>
     </row>
-    <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" customFormat="false" ht="729.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="s">
-        <v>3321</v>
+        <v>3323</v>
       </c>
       <c r="B261" s="5" t="s">
-        <v>3322</v>
+        <v>3296</v>
       </c>
       <c r="C261" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D261" s="5" t="s">
-        <v>3323</v>
-      </c>
-      <c r="E261" s="5" t="n">
-        <v>3</v>
+        <v>3296</v>
+      </c>
+      <c r="E261" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F261" s="5" t="n">
-        <v>2017</v>
+        <v>2011</v>
       </c>
       <c r="G261" s="5" t="s">
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="H261" s="5" t="s">
-        <v>3324</v>
+        <v>815</v>
       </c>
       <c r="I261" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J261" s="5" t="s">
+        <v>3311</v>
+      </c>
+      <c r="K261" s="5" t="s">
+        <v>3324</v>
+      </c>
+      <c r="L261" s="5" t="s">
         <v>3325</v>
       </c>
-      <c r="K261" s="5" t="s">
+      <c r="M261" s="5" t="s">
         <v>3326</v>
       </c>
-      <c r="L261" s="5" t="s">
+      <c r="N261" s="5" t="s">
         <v>3327</v>
       </c>
-      <c r="M261" s="5" t="s">
+      <c r="O261" s="5" t="s">
         <v>3328</v>
       </c>
-      <c r="N261" s="5" t="s">
+      <c r="P261" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q261" s="5" t="s">
         <v>3329</v>
       </c>
-      <c r="O261" s="5" t="s">
+      <c r="R261" s="5" t="s">
         <v>3330</v>
       </c>
-      <c r="P261" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="Q261" s="5" t="s">
+      <c r="S261" s="5" t="s">
         <v>3331</v>
       </c>
-      <c r="R261" s="5" t="s">
+      <c r="T261" s="5" t="s">
         <v>3332</v>
       </c>
-      <c r="S261" s="5" t="s">
+      <c r="U261" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="V261" s="8" t="s">
         <v>3333</v>
-      </c>
-      <c r="T261" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="U261" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="V261" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="W261" s="5" t="s">
         <v>3334</v>
@@ -29965,52 +30007,52 @@
         <v>25</v>
       </c>
       <c r="D262" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E262" s="5" t="s">
-        <v>26</v>
+        <v>3337</v>
+      </c>
+      <c r="E262" s="5" t="n">
+        <v>3</v>
       </c>
       <c r="F262" s="5" t="n">
-        <v>1990</v>
+        <v>2017</v>
       </c>
       <c r="G262" s="5" t="s">
-        <v>27</v>
+        <v>117</v>
       </c>
       <c r="H262" s="5" t="s">
-        <v>3337</v>
+        <v>3338</v>
       </c>
       <c r="I262" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J262" s="5" t="s">
-        <v>1027</v>
+        <v>3339</v>
       </c>
       <c r="K262" s="5" t="s">
-        <v>2827</v>
+        <v>3340</v>
       </c>
       <c r="L262" s="5" t="s">
-        <v>3338</v>
+        <v>3341</v>
       </c>
       <c r="M262" s="5" t="s">
-        <v>3339</v>
+        <v>3342</v>
       </c>
       <c r="N262" s="5" t="s">
-        <v>3340</v>
+        <v>3343</v>
       </c>
       <c r="O262" s="5" t="s">
-        <v>3341</v>
+        <v>3344</v>
       </c>
       <c r="P262" s="5" t="s">
-        <v>434</v>
+        <v>380</v>
       </c>
       <c r="Q262" s="5" t="s">
-        <v>3342</v>
+        <v>3345</v>
       </c>
       <c r="R262" s="5" t="s">
-        <v>3343</v>
+        <v>3346</v>
       </c>
       <c r="S262" s="5" t="s">
-        <v>3344</v>
+        <v>3347</v>
       </c>
       <c r="T262" s="5" t="s">
         <v>106</v>
@@ -30022,16 +30064,16 @@
         <v>106</v>
       </c>
       <c r="W262" s="5" t="s">
-        <v>3345</v>
+        <v>3348</v>
       </c>
       <c r="X262" s="5"/>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="s">
-        <v>3346</v>
+        <v>3349</v>
       </c>
       <c r="B263" s="5" t="s">
-        <v>3347</v>
+        <v>3350</v>
       </c>
       <c r="C263" s="5" t="s">
         <v>25</v>
@@ -30046,43 +30088,43 @@
         <v>1990</v>
       </c>
       <c r="G263" s="5" t="s">
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="H263" s="5" t="s">
-        <v>1971</v>
+        <v>3351</v>
       </c>
       <c r="I263" s="5" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="J263" s="5" t="s">
-        <v>3348</v>
+        <v>1027</v>
       </c>
       <c r="K263" s="5" t="s">
-        <v>3349</v>
+        <v>2827</v>
       </c>
       <c r="L263" s="5" t="s">
-        <v>3350</v>
+        <v>3352</v>
       </c>
       <c r="M263" s="5" t="s">
-        <v>3351</v>
+        <v>3353</v>
       </c>
       <c r="N263" s="5" t="s">
-        <v>3352</v>
+        <v>3354</v>
       </c>
       <c r="O263" s="5" t="s">
-        <v>3353</v>
+        <v>3355</v>
       </c>
       <c r="P263" s="5" t="s">
-        <v>71</v>
+        <v>434</v>
       </c>
       <c r="Q263" s="5" t="s">
-        <v>3354</v>
+        <v>3356</v>
       </c>
       <c r="R263" s="5" t="s">
-        <v>3355</v>
+        <v>3357</v>
       </c>
       <c r="S263" s="5" t="s">
-        <v>3356</v>
+        <v>3358</v>
       </c>
       <c r="T263" s="5" t="s">
         <v>106</v>
@@ -30094,160 +30136,160 @@
         <v>106</v>
       </c>
       <c r="W263" s="5" t="s">
-        <v>3357</v>
+        <v>3359</v>
       </c>
       <c r="X263" s="5"/>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="s">
-        <v>3358</v>
+        <v>3360</v>
       </c>
       <c r="B264" s="5" t="s">
-        <v>3359</v>
+        <v>3361</v>
       </c>
       <c r="C264" s="5" t="s">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="D264" s="5" t="s">
-        <v>3360</v>
+        <v>26</v>
       </c>
       <c r="E264" s="5" t="s">
-        <v>3361</v>
+        <v>26</v>
       </c>
       <c r="F264" s="5" t="n">
-        <v>1961</v>
+        <v>1990</v>
       </c>
       <c r="G264" s="5" t="s">
-        <v>2094</v>
+        <v>117</v>
       </c>
       <c r="H264" s="5" t="s">
+        <v>1971</v>
+      </c>
+      <c r="I264" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J264" s="5" t="s">
         <v>3362</v>
       </c>
-      <c r="I264" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J264" s="5" t="s">
+      <c r="K264" s="5" t="s">
         <v>3363</v>
       </c>
-      <c r="K264" s="5" t="s">
+      <c r="L264" s="5" t="s">
         <v>3364</v>
       </c>
-      <c r="L264" s="5" t="s">
+      <c r="M264" s="5" t="s">
         <v>3365</v>
       </c>
-      <c r="M264" s="5" t="s">
+      <c r="N264" s="5" t="s">
         <v>3366</v>
       </c>
-      <c r="N264" s="5" t="s">
+      <c r="O264" s="5" t="s">
         <v>3367</v>
       </c>
-      <c r="O264" s="5" t="s">
+      <c r="P264" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q264" s="5" t="s">
         <v>3368</v>
       </c>
-      <c r="P264" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="Q264" s="5" t="s">
+      <c r="R264" s="5" t="s">
         <v>3369</v>
-      </c>
-      <c r="R264" s="5" t="s">
-        <v>2707</v>
       </c>
       <c r="S264" s="5" t="s">
         <v>3370</v>
       </c>
-      <c r="T264" s="10" t="s">
+      <c r="T264" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="U264" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="V264" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="W264" s="5" t="s">
         <v>3371</v>
-      </c>
-      <c r="U264" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="V264" s="5" t="s">
-        <v>3372</v>
-      </c>
-      <c r="W264" s="5" t="s">
-        <v>3373</v>
       </c>
       <c r="X264" s="5"/>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
+        <v>3372</v>
+      </c>
+      <c r="B265" s="5" t="s">
+        <v>3373</v>
+      </c>
+      <c r="C265" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D265" s="5" t="s">
         <v>3374</v>
       </c>
-      <c r="B265" s="5" t="s">
+      <c r="E265" s="5" t="s">
         <v>3375</v>
       </c>
-      <c r="C265" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D265" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E265" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="F265" s="5" t="n">
-        <v>2018</v>
+        <v>1961</v>
       </c>
       <c r="G265" s="5" t="s">
-        <v>27</v>
+        <v>2094</v>
       </c>
       <c r="H265" s="5" t="s">
-        <v>2159</v>
+        <v>3376</v>
       </c>
       <c r="I265" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J265" s="5" t="s">
-        <v>984</v>
+        <v>3377</v>
       </c>
       <c r="K265" s="5" t="s">
-        <v>3376</v>
+        <v>3378</v>
       </c>
       <c r="L265" s="5" t="s">
-        <v>3377</v>
+        <v>3379</v>
       </c>
       <c r="M265" s="5" t="s">
-        <v>3378</v>
+        <v>3380</v>
       </c>
       <c r="N265" s="5" t="s">
-        <v>3379</v>
+        <v>3381</v>
       </c>
       <c r="O265" s="5" t="s">
-        <v>3380</v>
+        <v>3382</v>
       </c>
       <c r="P265" s="5" t="s">
-        <v>434</v>
+        <v>462</v>
       </c>
       <c r="Q265" s="5" t="s">
-        <v>3381</v>
+        <v>3383</v>
       </c>
       <c r="R265" s="5" t="s">
-        <v>38</v>
+        <v>2707</v>
       </c>
       <c r="S265" s="5" t="s">
-        <v>3382</v>
-      </c>
-      <c r="T265" s="5" t="s">
-        <v>106</v>
+        <v>3384</v>
+      </c>
+      <c r="T265" s="10" t="s">
+        <v>3385</v>
       </c>
       <c r="U265" s="5" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="V265" s="5" t="s">
-        <v>106</v>
+        <v>3386</v>
       </c>
       <c r="W265" s="5" t="s">
-        <v>3383</v>
+        <v>3387</v>
       </c>
       <c r="X265" s="5"/>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="s">
-        <v>3384</v>
+        <v>3388</v>
       </c>
       <c r="B266" s="5" t="s">
-        <v>3385</v>
+        <v>3389</v>
       </c>
       <c r="C266" s="5" t="s">
         <v>25</v>
@@ -30259,55 +30301,55 @@
         <v>26</v>
       </c>
       <c r="F266" s="5" t="n">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="G266" s="5" t="s">
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="H266" s="5" t="s">
-        <v>1493</v>
+        <v>2159</v>
       </c>
       <c r="I266" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J266" s="5" t="s">
-        <v>3386</v>
+        <v>984</v>
       </c>
       <c r="K266" s="5" t="s">
-        <v>3387</v>
+        <v>3390</v>
       </c>
       <c r="L266" s="5" t="s">
-        <v>3388</v>
+        <v>3391</v>
       </c>
       <c r="M266" s="5" t="s">
-        <v>3389</v>
+        <v>3392</v>
       </c>
       <c r="N266" s="5" t="s">
-        <v>3390</v>
+        <v>3393</v>
       </c>
       <c r="O266" s="5" t="s">
-        <v>3391</v>
+        <v>3394</v>
       </c>
       <c r="P266" s="5" t="s">
-        <v>535</v>
+        <v>434</v>
       </c>
       <c r="Q266" s="5" t="s">
-        <v>3392</v>
+        <v>3395</v>
       </c>
       <c r="R266" s="5" t="s">
-        <v>3393</v>
+        <v>38</v>
       </c>
       <c r="S266" s="5" t="s">
-        <v>3394</v>
+        <v>3396</v>
       </c>
       <c r="T266" s="5" t="s">
-        <v>3395</v>
+        <v>106</v>
       </c>
       <c r="U266" s="5" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="V266" s="5" t="s">
-        <v>3396</v>
+        <v>106</v>
       </c>
       <c r="W266" s="5" t="s">
         <v>3397</v>
@@ -30325,124 +30367,124 @@
         <v>25</v>
       </c>
       <c r="D267" s="5" t="s">
-        <v>1444</v>
+        <v>26</v>
       </c>
       <c r="E267" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F267" s="5" t="n">
-        <v>2015</v>
+        <v>2008</v>
       </c>
       <c r="G267" s="5" t="s">
-        <v>27</v>
+        <v>117</v>
       </c>
       <c r="H267" s="5" t="s">
+        <v>1493</v>
+      </c>
+      <c r="I267" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J267" s="5" t="s">
         <v>3400</v>
       </c>
-      <c r="I267" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J267" s="5" t="s">
+      <c r="K267" s="5" t="s">
         <v>3401</v>
       </c>
-      <c r="K267" s="5" t="s">
+      <c r="L267" s="5" t="s">
         <v>3402</v>
       </c>
-      <c r="L267" s="5" t="s">
+      <c r="M267" s="5" t="s">
         <v>3403</v>
       </c>
-      <c r="M267" s="5" t="s">
+      <c r="N267" s="5" t="s">
         <v>3404</v>
       </c>
-      <c r="N267" s="5" t="s">
+      <c r="O267" s="5" t="s">
         <v>3405</v>
       </c>
-      <c r="O267" s="5" t="s">
+      <c r="P267" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="Q267" s="5" t="s">
         <v>3406</v>
       </c>
-      <c r="P267" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q267" s="5" t="s">
+      <c r="R267" s="5" t="s">
         <v>3407</v>
       </c>
-      <c r="R267" s="5" t="s">
+      <c r="S267" s="5" t="s">
         <v>3408</v>
       </c>
-      <c r="S267" s="5" t="s">
+      <c r="T267" s="5" t="s">
         <v>3409</v>
       </c>
-      <c r="T267" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="U267" s="5" t="s">
-        <v>106</v>
+        <v>41</v>
       </c>
       <c r="V267" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="W267" s="4" t="s">
         <v>3410</v>
       </c>
-      <c r="X267" s="4"/>
+      <c r="W267" s="5" t="s">
+        <v>3411</v>
+      </c>
+      <c r="X267" s="5"/>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="s">
-        <v>3411</v>
+        <v>3412</v>
       </c>
       <c r="B268" s="5" t="s">
-        <v>3412</v>
+        <v>3413</v>
       </c>
       <c r="C268" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D268" s="5" t="s">
-        <v>26</v>
+        <v>1444</v>
       </c>
       <c r="E268" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F268" s="5" t="n">
-        <v>2008</v>
+        <v>2015</v>
       </c>
       <c r="G268" s="5" t="s">
-        <v>285</v>
+        <v>27</v>
       </c>
       <c r="H268" s="5" t="s">
-        <v>2197</v>
+        <v>3414</v>
       </c>
       <c r="I268" s="5" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="J268" s="5" t="s">
-        <v>3413</v>
+        <v>3415</v>
       </c>
       <c r="K268" s="5" t="s">
-        <v>3414</v>
+        <v>3416</v>
       </c>
       <c r="L268" s="5" t="s">
-        <v>3415</v>
+        <v>3417</v>
       </c>
       <c r="M268" s="5" t="s">
-        <v>3416</v>
+        <v>3418</v>
       </c>
       <c r="N268" s="5" t="s">
-        <v>3417</v>
+        <v>3419</v>
       </c>
       <c r="O268" s="5" t="s">
-        <v>3418</v>
+        <v>3420</v>
       </c>
       <c r="P268" s="5" t="s">
-        <v>220</v>
+        <v>157</v>
       </c>
       <c r="Q268" s="5" t="s">
-        <v>3419</v>
+        <v>3421</v>
       </c>
       <c r="R268" s="5" t="s">
-        <v>3420</v>
+        <v>3422</v>
       </c>
       <c r="S268" s="5" t="s">
-        <v>3421</v>
+        <v>3423</v>
       </c>
       <c r="T268" s="5" t="s">
         <v>106</v>
@@ -30453,17 +30495,17 @@
       <c r="V268" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="W268" s="5" t="s">
-        <v>3422</v>
-      </c>
-      <c r="X268" s="5"/>
+      <c r="W268" s="4" t="s">
+        <v>3424</v>
+      </c>
+      <c r="X268" s="4"/>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="s">
-        <v>3423</v>
+        <v>3425</v>
       </c>
       <c r="B269" s="5" t="s">
-        <v>3424</v>
+        <v>3426</v>
       </c>
       <c r="C269" s="5" t="s">
         <v>25</v>
@@ -30475,46 +30517,46 @@
         <v>26</v>
       </c>
       <c r="F269" s="5" t="n">
-        <v>1979</v>
+        <v>2008</v>
       </c>
       <c r="G269" s="5" t="s">
-        <v>27</v>
+        <v>285</v>
       </c>
       <c r="H269" s="5" t="s">
-        <v>3425</v>
+        <v>2197</v>
       </c>
       <c r="I269" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J269" s="5" t="s">
-        <v>638</v>
+        <v>3427</v>
       </c>
       <c r="K269" s="5" t="s">
-        <v>3426</v>
+        <v>3428</v>
       </c>
       <c r="L269" s="5" t="s">
-        <v>3427</v>
+        <v>3429</v>
       </c>
       <c r="M269" s="5" t="s">
-        <v>3428</v>
+        <v>3430</v>
       </c>
       <c r="N269" s="5" t="s">
-        <v>3429</v>
+        <v>3431</v>
       </c>
       <c r="O269" s="5" t="s">
-        <v>3430</v>
+        <v>3432</v>
       </c>
       <c r="P269" s="5" t="s">
-        <v>434</v>
+        <v>220</v>
       </c>
       <c r="Q269" s="5" t="s">
-        <v>3431</v>
+        <v>3433</v>
       </c>
       <c r="R269" s="5" t="s">
-        <v>38</v>
+        <v>3434</v>
       </c>
       <c r="S269" s="5" t="s">
-        <v>3432</v>
+        <v>3435</v>
       </c>
       <c r="T269" s="5" t="s">
         <v>106</v>
@@ -30526,31 +30568,31 @@
         <v>106</v>
       </c>
       <c r="W269" s="5" t="s">
-        <v>3433</v>
+        <v>3436</v>
       </c>
       <c r="X269" s="5"/>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="s">
-        <v>3434</v>
+        <v>3437</v>
       </c>
       <c r="B270" s="5" t="s">
-        <v>3435</v>
+        <v>3438</v>
       </c>
       <c r="C270" s="5" t="s">
-        <v>3436</v>
+        <v>25</v>
       </c>
       <c r="D270" s="5" t="s">
-        <v>3437</v>
+        <v>26</v>
       </c>
       <c r="E270" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F270" s="5" t="n">
-        <v>2008</v>
+        <v>1979</v>
       </c>
       <c r="G270" s="5" t="s">
-        <v>3438</v>
+        <v>27</v>
       </c>
       <c r="H270" s="5" t="s">
         <v>3439</v>
@@ -30559,34 +30601,34 @@
         <v>29</v>
       </c>
       <c r="J270" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="K270" s="5" t="s">
         <v>3440</v>
       </c>
-      <c r="K270" s="5" t="s">
+      <c r="L270" s="5" t="s">
         <v>3441</v>
       </c>
-      <c r="L270" s="5" t="s">
+      <c r="M270" s="5" t="s">
         <v>3442</v>
       </c>
-      <c r="M270" s="5" t="s">
+      <c r="N270" s="5" t="s">
         <v>3443</v>
       </c>
-      <c r="N270" s="5" t="s">
+      <c r="O270" s="5" t="s">
         <v>3444</v>
       </c>
-      <c r="O270" s="5" t="s">
+      <c r="P270" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="Q270" s="5" t="s">
         <v>3445</v>
       </c>
-      <c r="P270" s="5" t="s">
-        <v>1186</v>
-      </c>
-      <c r="Q270" s="5" t="s">
+      <c r="R270" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="S270" s="5" t="s">
         <v>3446</v>
-      </c>
-      <c r="R270" s="5" t="s">
-        <v>2278</v>
-      </c>
-      <c r="S270" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="T270" s="5" t="s">
         <v>106</v>
@@ -30610,55 +30652,55 @@
         <v>3449</v>
       </c>
       <c r="C271" s="5" t="s">
-        <v>25</v>
+        <v>3450</v>
       </c>
       <c r="D271" s="5" t="s">
-        <v>26</v>
+        <v>3451</v>
       </c>
       <c r="E271" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F271" s="5" t="n">
-        <v>1988</v>
+        <v>2008</v>
       </c>
       <c r="G271" s="5" t="s">
-        <v>331</v>
+        <v>3452</v>
       </c>
       <c r="H271" s="5" t="s">
-        <v>2838</v>
+        <v>3453</v>
       </c>
       <c r="I271" s="5" t="s">
-        <v>1367</v>
+        <v>29</v>
       </c>
       <c r="J271" s="5" t="s">
-        <v>3450</v>
+        <v>3454</v>
       </c>
       <c r="K271" s="5" t="s">
-        <v>861</v>
+        <v>3455</v>
       </c>
       <c r="L271" s="5" t="s">
-        <v>3451</v>
+        <v>3456</v>
       </c>
       <c r="M271" s="5" t="s">
-        <v>3452</v>
+        <v>3457</v>
       </c>
       <c r="N271" s="5" t="s">
-        <v>3453</v>
+        <v>3458</v>
       </c>
       <c r="O271" s="5" t="s">
-        <v>3454</v>
+        <v>3459</v>
       </c>
       <c r="P271" s="5" t="s">
-        <v>338</v>
+        <v>1186</v>
       </c>
       <c r="Q271" s="5" t="s">
-        <v>3455</v>
+        <v>3460</v>
       </c>
       <c r="R271" s="5" t="s">
-        <v>174</v>
+        <v>2278</v>
       </c>
       <c r="S271" s="5" t="s">
-        <v>3456</v>
+        <v>106</v>
       </c>
       <c r="T271" s="5" t="s">
         <v>106</v>
@@ -30670,16 +30712,16 @@
         <v>106</v>
       </c>
       <c r="W271" s="5" t="s">
-        <v>3457</v>
+        <v>3461</v>
       </c>
       <c r="X271" s="5"/>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="s">
-        <v>3458</v>
+        <v>3462</v>
       </c>
       <c r="B272" s="5" t="s">
-        <v>3459</v>
+        <v>3463</v>
       </c>
       <c r="C272" s="5" t="s">
         <v>25</v>
@@ -30691,46 +30733,46 @@
         <v>26</v>
       </c>
       <c r="F272" s="5" t="n">
-        <v>1971</v>
+        <v>1988</v>
       </c>
       <c r="G272" s="5" t="s">
-        <v>285</v>
+        <v>331</v>
       </c>
       <c r="H272" s="5" t="s">
-        <v>2159</v>
+        <v>2838</v>
       </c>
       <c r="I272" s="5" t="s">
-        <v>29</v>
+        <v>1367</v>
       </c>
       <c r="J272" s="5" t="s">
-        <v>3460</v>
+        <v>3464</v>
       </c>
       <c r="K272" s="5" t="s">
-        <v>3461</v>
+        <v>861</v>
       </c>
       <c r="L272" s="5" t="s">
-        <v>3462</v>
+        <v>3465</v>
       </c>
       <c r="M272" s="5" t="s">
-        <v>3463</v>
+        <v>3466</v>
       </c>
       <c r="N272" s="5" t="s">
-        <v>3464</v>
+        <v>3467</v>
       </c>
       <c r="O272" s="5" t="s">
-        <v>3465</v>
+        <v>3468</v>
       </c>
       <c r="P272" s="5" t="s">
-        <v>107</v>
+        <v>338</v>
       </c>
       <c r="Q272" s="5" t="s">
-        <v>3466</v>
+        <v>3469</v>
       </c>
       <c r="R272" s="5" t="s">
-        <v>3097</v>
+        <v>174</v>
       </c>
       <c r="S272" s="5" t="s">
-        <v>3467</v>
+        <v>3470</v>
       </c>
       <c r="T272" s="5" t="s">
         <v>106</v>
@@ -30742,211 +30784,211 @@
         <v>106</v>
       </c>
       <c r="W272" s="5" t="s">
-        <v>3468</v>
+        <v>3471</v>
       </c>
       <c r="X272" s="5"/>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="s">
-        <v>3469</v>
+        <v>3472</v>
       </c>
       <c r="B273" s="5" t="s">
-        <v>3470</v>
+        <v>3473</v>
       </c>
       <c r="C273" s="5" t="s">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="D273" s="5" t="s">
-        <v>3471</v>
+        <v>26</v>
       </c>
       <c r="E273" s="5" t="s">
-        <v>3472</v>
+        <v>26</v>
       </c>
       <c r="F273" s="5" t="n">
-        <v>2002</v>
+        <v>1971</v>
       </c>
       <c r="G273" s="5" t="s">
-        <v>487</v>
+        <v>285</v>
       </c>
       <c r="H273" s="5" t="s">
-        <v>3473</v>
+        <v>2159</v>
       </c>
       <c r="I273" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J273" s="5" t="s">
-        <v>612</v>
+        <v>3474</v>
       </c>
       <c r="K273" s="5" t="s">
-        <v>3474</v>
+        <v>3475</v>
       </c>
       <c r="L273" s="5" t="s">
-        <v>3475</v>
+        <v>3476</v>
       </c>
       <c r="M273" s="5" t="s">
-        <v>3476</v>
+        <v>3477</v>
       </c>
       <c r="N273" s="5" t="s">
-        <v>3477</v>
+        <v>3478</v>
       </c>
       <c r="O273" s="5" t="s">
-        <v>3478</v>
+        <v>3479</v>
       </c>
       <c r="P273" s="5" t="s">
-        <v>3479</v>
+        <v>107</v>
       </c>
       <c r="Q273" s="5" t="s">
         <v>3480</v>
       </c>
       <c r="R273" s="5" t="s">
+        <v>3097</v>
+      </c>
+      <c r="S273" s="5" t="s">
         <v>3481</v>
       </c>
-      <c r="S273" s="5" t="s">
+      <c r="T273" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="U273" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="V273" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="W273" s="5" t="s">
         <v>3482</v>
-      </c>
-      <c r="T273" s="5" t="s">
-        <v>3483</v>
-      </c>
-      <c r="U273" s="5" t="s">
-        <v>3484</v>
-      </c>
-      <c r="V273" s="5" t="s">
-        <v>3485</v>
-      </c>
-      <c r="W273" s="5" t="s">
-        <v>3486</v>
       </c>
       <c r="X273" s="5"/>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="s">
+        <v>3483</v>
+      </c>
+      <c r="B274" s="5" t="s">
+        <v>3484</v>
+      </c>
+      <c r="C274" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D274" s="5" t="s">
+        <v>3485</v>
+      </c>
+      <c r="E274" s="5" t="s">
+        <v>3486</v>
+      </c>
+      <c r="F274" s="5" t="n">
+        <v>2002</v>
+      </c>
+      <c r="G274" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="H274" s="5" t="s">
         <v>3487</v>
       </c>
-      <c r="B274" s="5" t="s">
+      <c r="I274" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J274" s="5" t="s">
+        <v>612</v>
+      </c>
+      <c r="K274" s="5" t="s">
         <v>3488</v>
       </c>
-      <c r="C274" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D274" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E274" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F274" s="5" t="n">
-        <v>2017</v>
-      </c>
-      <c r="G274" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="H274" s="5" t="s">
+      <c r="L274" s="5" t="s">
         <v>3489</v>
       </c>
-      <c r="I274" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J274" s="5" t="s">
+      <c r="M274" s="5" t="s">
         <v>3490</v>
       </c>
-      <c r="K274" s="5" t="s">
+      <c r="N274" s="5" t="s">
         <v>3491</v>
       </c>
-      <c r="L274" s="5" t="s">
+      <c r="O274" s="5" t="s">
         <v>3492</v>
       </c>
-      <c r="M274" s="5" t="s">
+      <c r="P274" s="5" t="s">
         <v>3493</v>
       </c>
-      <c r="N274" s="5" t="s">
+      <c r="Q274" s="5" t="s">
         <v>3494</v>
       </c>
-      <c r="O274" s="5" t="s">
+      <c r="R274" s="5" t="s">
         <v>3495</v>
       </c>
-      <c r="P274" s="5" t="s">
-        <v>1267</v>
-      </c>
-      <c r="Q274" s="5" t="s">
+      <c r="S274" s="5" t="s">
         <v>3496</v>
       </c>
-      <c r="R274" s="5" t="s">
+      <c r="T274" s="5" t="s">
         <v>3497</v>
       </c>
-      <c r="S274" s="5" t="s">
+      <c r="U274" s="5" t="s">
         <v>3498</v>
       </c>
-      <c r="T274" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="U274" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="V274" s="5" t="s">
-        <v>106</v>
+        <v>3499</v>
       </c>
       <c r="W274" s="5" t="s">
-        <v>3499</v>
+        <v>3500</v>
       </c>
       <c r="X274" s="5"/>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
-        <v>3500</v>
+        <v>3501</v>
       </c>
       <c r="B275" s="5" t="s">
-        <v>3501</v>
+        <v>3502</v>
       </c>
       <c r="C275" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D275" s="5" t="s">
-        <v>1444</v>
+        <v>26</v>
       </c>
       <c r="E275" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F275" s="5" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="G275" s="5" t="s">
-        <v>27</v>
+        <v>117</v>
       </c>
       <c r="H275" s="5" t="s">
-        <v>2596</v>
+        <v>3503</v>
       </c>
       <c r="I275" s="5" t="s">
         <v>64</v>
       </c>
       <c r="J275" s="5" t="s">
-        <v>3502</v>
+        <v>3504</v>
       </c>
       <c r="K275" s="5" t="s">
-        <v>3503</v>
+        <v>3505</v>
       </c>
       <c r="L275" s="5" t="s">
-        <v>3504</v>
+        <v>3506</v>
       </c>
       <c r="M275" s="5" t="s">
-        <v>3505</v>
+        <v>3507</v>
       </c>
       <c r="N275" s="5" t="s">
-        <v>3506</v>
+        <v>3508</v>
       </c>
       <c r="O275" s="5" t="s">
-        <v>3507</v>
+        <v>3509</v>
       </c>
       <c r="P275" s="5" t="s">
-        <v>306</v>
+        <v>1267</v>
       </c>
       <c r="Q275" s="5" t="s">
-        <v>3508</v>
+        <v>3510</v>
       </c>
       <c r="R275" s="5" t="s">
-        <v>2324</v>
+        <v>3511</v>
       </c>
       <c r="S275" s="5" t="s">
-        <v>3509</v>
+        <v>3512</v>
       </c>
       <c r="T275" s="5" t="s">
         <v>106</v>
@@ -30957,68 +30999,68 @@
       <c r="V275" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="W275" s="4" t="s">
-        <v>3510</v>
-      </c>
-      <c r="X275" s="4"/>
+      <c r="W275" s="5" t="s">
+        <v>3513</v>
+      </c>
+      <c r="X275" s="5"/>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
-        <v>3511</v>
+        <v>3514</v>
       </c>
       <c r="B276" s="5" t="s">
-        <v>3512</v>
+        <v>3515</v>
       </c>
       <c r="C276" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D276" s="5" t="s">
-        <v>3512</v>
-      </c>
-      <c r="E276" s="6" t="n">
-        <v>1</v>
+        <v>1444</v>
+      </c>
+      <c r="E276" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="F276" s="5" t="n">
-        <v>2000</v>
+        <v>2022</v>
       </c>
       <c r="G276" s="5" t="s">
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="H276" s="5" t="s">
-        <v>2838</v>
+        <v>2596</v>
       </c>
       <c r="I276" s="5" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="J276" s="5" t="s">
-        <v>1027</v>
+        <v>3516</v>
       </c>
       <c r="K276" s="5" t="s">
-        <v>3387</v>
+        <v>3517</v>
       </c>
       <c r="L276" s="5" t="s">
-        <v>3513</v>
+        <v>3518</v>
       </c>
       <c r="M276" s="5" t="s">
-        <v>3514</v>
+        <v>3519</v>
       </c>
       <c r="N276" s="5" t="s">
-        <v>3515</v>
+        <v>3520</v>
       </c>
       <c r="O276" s="5" t="s">
-        <v>3516</v>
+        <v>3521</v>
       </c>
       <c r="P276" s="5" t="s">
-        <v>1267</v>
+        <v>306</v>
       </c>
       <c r="Q276" s="5" t="s">
-        <v>3517</v>
+        <v>3522</v>
       </c>
       <c r="R276" s="5" t="s">
-        <v>3518</v>
+        <v>2324</v>
       </c>
       <c r="S276" s="5" t="s">
-        <v>3519</v>
+        <v>3523</v>
       </c>
       <c r="T276" s="5" t="s">
         <v>106</v>
@@ -31029,68 +31071,68 @@
       <c r="V276" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="W276" s="5" t="s">
-        <v>3520</v>
-      </c>
-      <c r="X276" s="5"/>
+      <c r="W276" s="4" t="s">
+        <v>3524</v>
+      </c>
+      <c r="X276" s="4"/>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
-        <v>3521</v>
+        <v>3525</v>
       </c>
       <c r="B277" s="5" t="s">
-        <v>3522</v>
+        <v>3526</v>
       </c>
       <c r="C277" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D277" s="5" t="s">
-        <v>3512</v>
+        <v>3526</v>
       </c>
       <c r="E277" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F277" s="5" t="n">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="G277" s="5" t="s">
         <v>117</v>
       </c>
       <c r="H277" s="5" t="s">
-        <v>3523</v>
+        <v>2838</v>
       </c>
       <c r="I277" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J277" s="5" t="s">
-        <v>984</v>
+        <v>1027</v>
       </c>
       <c r="K277" s="5" t="s">
-        <v>3387</v>
+        <v>3401</v>
       </c>
       <c r="L277" s="5" t="s">
-        <v>3524</v>
+        <v>3527</v>
       </c>
       <c r="M277" s="5" t="s">
-        <v>3525</v>
+        <v>3528</v>
       </c>
       <c r="N277" s="5" t="s">
-        <v>3526</v>
+        <v>3529</v>
       </c>
       <c r="O277" s="5" t="s">
-        <v>3527</v>
+        <v>3530</v>
       </c>
       <c r="P277" s="5" t="s">
-        <v>644</v>
+        <v>1267</v>
       </c>
       <c r="Q277" s="5" t="s">
-        <v>3528</v>
+        <v>3531</v>
       </c>
       <c r="R277" s="5" t="s">
-        <v>3529</v>
+        <v>3532</v>
       </c>
       <c r="S277" s="5" t="s">
-        <v>3530</v>
+        <v>3533</v>
       </c>
       <c r="T277" s="5" t="s">
         <v>106</v>
@@ -31102,67 +31144,67 @@
         <v>106</v>
       </c>
       <c r="W277" s="5" t="s">
-        <v>3531</v>
+        <v>3534</v>
       </c>
       <c r="X277" s="5"/>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
-        <v>3532</v>
+        <v>3535</v>
       </c>
       <c r="B278" s="5" t="s">
-        <v>3533</v>
+        <v>3536</v>
       </c>
       <c r="C278" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D278" s="5" t="s">
-        <v>3512</v>
-      </c>
-      <c r="E278" s="6" t="s">
-        <v>26</v>
+        <v>3526</v>
+      </c>
+      <c r="E278" s="6" t="n">
+        <v>2</v>
       </c>
       <c r="F278" s="5" t="n">
-        <v>2017</v>
+        <v>2003</v>
       </c>
       <c r="G278" s="5" t="s">
-        <v>27</v>
+        <v>117</v>
       </c>
       <c r="H278" s="5" t="s">
-        <v>1840</v>
+        <v>3537</v>
       </c>
       <c r="I278" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J278" s="5" t="s">
-        <v>582</v>
+        <v>984</v>
       </c>
       <c r="K278" s="5" t="s">
-        <v>82</v>
+        <v>3401</v>
       </c>
       <c r="L278" s="5" t="s">
-        <v>3534</v>
+        <v>3538</v>
       </c>
       <c r="M278" s="5" t="s">
-        <v>3535</v>
+        <v>3539</v>
       </c>
       <c r="N278" s="5" t="s">
-        <v>3536</v>
+        <v>3540</v>
       </c>
       <c r="O278" s="5" t="s">
-        <v>3537</v>
+        <v>3541</v>
       </c>
       <c r="P278" s="5" t="s">
-        <v>476</v>
+        <v>644</v>
       </c>
       <c r="Q278" s="5" t="s">
-        <v>3538</v>
+        <v>3542</v>
       </c>
       <c r="R278" s="5" t="s">
-        <v>3539</v>
+        <v>3543</v>
       </c>
       <c r="S278" s="5" t="s">
-        <v>3540</v>
+        <v>3544</v>
       </c>
       <c r="T278" s="5" t="s">
         <v>106</v>
@@ -31174,67 +31216,67 @@
         <v>106</v>
       </c>
       <c r="W278" s="5" t="s">
-        <v>3541</v>
+        <v>3545</v>
       </c>
       <c r="X278" s="5"/>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
-        <v>3542</v>
+        <v>3546</v>
       </c>
       <c r="B279" s="5" t="s">
-        <v>3543</v>
+        <v>3547</v>
       </c>
       <c r="C279" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D279" s="5" t="s">
+        <v>3526</v>
+      </c>
+      <c r="E279" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E279" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="F279" s="5" t="n">
-        <v>2009</v>
+        <v>2017</v>
       </c>
       <c r="G279" s="5" t="s">
         <v>27</v>
       </c>
       <c r="H279" s="5" t="s">
-        <v>1959</v>
+        <v>1840</v>
       </c>
       <c r="I279" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J279" s="5" t="s">
-        <v>3544</v>
+        <v>582</v>
       </c>
       <c r="K279" s="5" t="s">
-        <v>3545</v>
+        <v>82</v>
       </c>
       <c r="L279" s="5" t="s">
-        <v>3546</v>
+        <v>3548</v>
       </c>
       <c r="M279" s="5" t="s">
-        <v>3547</v>
+        <v>3549</v>
       </c>
       <c r="N279" s="5" t="s">
-        <v>3548</v>
+        <v>3550</v>
       </c>
       <c r="O279" s="5" t="s">
-        <v>3549</v>
+        <v>3551</v>
       </c>
       <c r="P279" s="5" t="s">
-        <v>434</v>
+        <v>476</v>
       </c>
       <c r="Q279" s="5" t="s">
-        <v>3550</v>
+        <v>3552</v>
       </c>
       <c r="R279" s="5" t="s">
-        <v>89</v>
+        <v>3553</v>
       </c>
       <c r="S279" s="5" t="s">
-        <v>3551</v>
+        <v>3554</v>
       </c>
       <c r="T279" s="5" t="s">
         <v>106</v>
@@ -31246,16 +31288,16 @@
         <v>106</v>
       </c>
       <c r="W279" s="5" t="s">
-        <v>3552</v>
+        <v>3555</v>
       </c>
       <c r="X279" s="5"/>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="s">
-        <v>3553</v>
+        <v>3556</v>
       </c>
       <c r="B280" s="5" t="s">
-        <v>3554</v>
+        <v>3557</v>
       </c>
       <c r="C280" s="5" t="s">
         <v>25</v>
@@ -31267,46 +31309,46 @@
         <v>26</v>
       </c>
       <c r="F280" s="5" t="n">
-        <v>2001</v>
+        <v>2009</v>
       </c>
       <c r="G280" s="5" t="s">
         <v>27</v>
       </c>
       <c r="H280" s="5" t="s">
-        <v>2723</v>
+        <v>1959</v>
       </c>
       <c r="I280" s="5" t="s">
         <v>29</v>
       </c>
       <c r="J280" s="5" t="s">
-        <v>349</v>
+        <v>3558</v>
       </c>
       <c r="K280" s="5" t="s">
-        <v>3555</v>
+        <v>3559</v>
       </c>
       <c r="L280" s="5" t="s">
-        <v>3556</v>
+        <v>3560</v>
       </c>
       <c r="M280" s="5" t="s">
-        <v>3557</v>
+        <v>3561</v>
       </c>
       <c r="N280" s="5" t="s">
-        <v>3558</v>
+        <v>3562</v>
       </c>
       <c r="O280" s="5" t="s">
-        <v>3559</v>
+        <v>3563</v>
       </c>
       <c r="P280" s="5" t="s">
-        <v>306</v>
+        <v>434</v>
       </c>
       <c r="Q280" s="5" t="s">
-        <v>3560</v>
+        <v>3564</v>
       </c>
       <c r="R280" s="5" t="s">
-        <v>3561</v>
+        <v>89</v>
       </c>
       <c r="S280" s="5" t="s">
-        <v>3562</v>
+        <v>3565</v>
       </c>
       <c r="T280" s="5" t="s">
         <v>106</v>
@@ -31318,111 +31360,183 @@
         <v>106</v>
       </c>
       <c r="W280" s="5" t="s">
-        <v>3563</v>
+        <v>3566</v>
       </c>
       <c r="X280" s="5"/>
     </row>
-    <row r="281" customFormat="false" ht="47.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A281" s="14" t="s">
-        <v>3564</v>
-      </c>
-      <c r="B281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="E281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="G281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="H281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="I281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="J281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="K281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="L281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="M281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="N281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="O281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="P281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="R281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="S281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="T281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="U281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="V281" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="W281" s="14" t="s">
-        <v>106</v>
-      </c>
+    <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="1" t="s">
+        <v>3567</v>
+      </c>
+      <c r="B281" s="5" t="s">
+        <v>3568</v>
+      </c>
+      <c r="C281" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D281" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E281" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F281" s="5" t="n">
+        <v>2001</v>
+      </c>
+      <c r="G281" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H281" s="5" t="s">
+        <v>2723</v>
+      </c>
+      <c r="I281" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J281" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="K281" s="5" t="s">
+        <v>3569</v>
+      </c>
+      <c r="L281" s="5" t="s">
+        <v>3570</v>
+      </c>
+      <c r="M281" s="5" t="s">
+        <v>3571</v>
+      </c>
+      <c r="N281" s="5" t="s">
+        <v>3572</v>
+      </c>
+      <c r="O281" s="5" t="s">
+        <v>3573</v>
+      </c>
+      <c r="P281" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q281" s="5" t="s">
+        <v>3574</v>
+      </c>
+      <c r="R281" s="5" t="s">
+        <v>3575</v>
+      </c>
+      <c r="S281" s="5" t="s">
+        <v>3576</v>
+      </c>
+      <c r="T281" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="U281" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="V281" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="W281" s="5" t="s">
+        <v>3577</v>
+      </c>
+      <c r="X281" s="5"/>
     </row>
-    <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A283" s="15" t="s">
-        <v>3565</v>
-      </c>
-      <c r="B283" s="1" t="s">
-        <v>3566</v>
+    <row r="282" customFormat="false" ht="47.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A282" s="14" t="s">
+        <v>3578</v>
+      </c>
+      <c r="B282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="G282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="H282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="I282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="K282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="L282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="M282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="N282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="O282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="P282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="R282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="S282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="T282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="U282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="V282" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="W282" s="14" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A284" s="15" t="s">
-        <v>3567</v>
+        <v>3579</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>3568</v>
+        <v>3580</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A285" s="1" t="s">
-        <v>3569</v>
+      <c r="A285" s="15" t="s">
+        <v>3581</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>3570</v>
+        <v>3582</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A286" s="14" t="s">
-        <v>3571</v>
+      <c r="A286" s="1" t="s">
+        <v>3583</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>3572</v>
+        <v>3584</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A287" s="14" t="s">
+        <v>3585</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>3586</v>
       </c>
     </row>
   </sheetData>
@@ -31581,13 +31695,18 @@
     <hyperlink ref="T232" r:id="rId152" display="https://www.rogerebert.com/reviews/the-silence-of-the-lambs-1991"/>
     <hyperlink ref="W232" r:id="rId153" display="https://image.tmdb.org/t/p/w600_and_h900_bestv2/uS9m8OBk1A8eM9I042bx8XXpqAq.jpg"/>
     <hyperlink ref="W233" r:id="rId154" display="https://xl.movieposterdb.com/06_05/2002/0286106/xl_116531_0286106_64875aa4.jpg?v=2024-07-07%2004:58:53"/>
-    <hyperlink ref="N264" r:id="rId155" display="https://youtu.be/ORbseYAkzRM?si=Kmi9lVFsGOqGC0qF"/>
-    <hyperlink ref="Q264" r:id="rId156" display="https://www.imdb.com/title/tt0052520/?ref_=fn_all_ttl_1"/>
-    <hyperlink ref="S264" r:id="rId157" display="https://www.rottentomatoes.com/tv/the_twilight_zone"/>
-    <hyperlink ref="T264" r:id="rId158" display="https://www.rogerebert.com/features/the-metaphor-years-writing-lessons-from-the-twilight-zone"/>
-    <hyperlink ref="W264" r:id="rId159" display="https://image.tmdb.org/t/p/w600_and_h900_bestv2/coWkN4uvxP41T0JFZHttUhS2PBj.jpg"/>
-    <hyperlink ref="Q266" r:id="rId160" display="https://www.imdb.com/title/tt0985699/?ref_=fn_all_ttl_1"/>
-    <hyperlink ref="Q273" r:id="rId161" display="https://www.imdb.com/title/tt0306414/"/>
+    <hyperlink ref="N258" r:id="rId155" display="https://youtu.be/FeSLPELpMeM?si=HBmM3L7nAy4c-0nX"/>
+    <hyperlink ref="Q258" r:id="rId156" display="https://www.imdb.com/title/tt0469494/?ref_=nv_sr_srsg_0_tt_8_nm_0_in_0_q_there%2520will%2520b"/>
+    <hyperlink ref="S258" r:id="rId157" display="https://www.rottentomatoes.com/m/there_will_be_blood"/>
+    <hyperlink ref="T258" r:id="rId158" display="https://www.rogerebert.com/reviews/there-will-be-blood-2008"/>
+    <hyperlink ref="W258" r:id="rId159" display="https://image.tmdb.org/t/p/w600_and_h900_bestv2/4ayObDELZfIXxVviT4GKTNc81wl.jpg"/>
+    <hyperlink ref="N265" r:id="rId160" display="https://youtu.be/ORbseYAkzRM?si=Kmi9lVFsGOqGC0qF"/>
+    <hyperlink ref="Q265" r:id="rId161" display="https://www.imdb.com/title/tt0052520/?ref_=fn_all_ttl_1"/>
+    <hyperlink ref="S265" r:id="rId162" display="https://www.rottentomatoes.com/tv/the_twilight_zone"/>
+    <hyperlink ref="T265" r:id="rId163" display="https://www.rogerebert.com/features/the-metaphor-years-writing-lessons-from-the-twilight-zone"/>
+    <hyperlink ref="W265" r:id="rId164" display="https://image.tmdb.org/t/p/w600_and_h900_bestv2/coWkN4uvxP41T0JFZHttUhS2PBj.jpg"/>
+    <hyperlink ref="Q267" r:id="rId165" display="https://www.imdb.com/title/tt0985699/?ref_=fn_all_ttl_1"/>
+    <hyperlink ref="Q274" r:id="rId166" display="https://www.imdb.com/title/tt0306414/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>